<commit_message>
sn: update sct forms.
</commit_message>
<xml_diff>
--- a/Coverage Survey/Senegal/sn_sct_lf_2_couverture_202112.xlsx
+++ b/Coverage Survey/Senegal/sn_sct_lf_2_couverture_202112.xlsx
@@ -96,7 +96,7 @@
     <t>c_numero_participant</t>
   </si>
   <si>
-    <t>Code du participant</t>
+    <t>Numéro du participant</t>
   </si>
   <si>
     <t>Le numéro d'ordre du participant</t>
@@ -111,16 +111,16 @@
     <t>concat(${c_village_id},'-',${c_recorder_id},'-',${c_numero_participant})</t>
   </si>
   <si>
+    <t>select_one sexe</t>
+  </si>
+  <si>
+    <t>c_sexe</t>
+  </si>
+  <si>
+    <t>Sexe</t>
+  </si>
+  <si>
     <t>c_age</t>
-  </si>
-  <si>
-    <t>Sexe</t>
-  </si>
-  <si>
-    <t>select_one sexe</t>
-  </si>
-  <si>
-    <t>c_sexe</t>
   </si>
   <si>
     <t>Age</t>
@@ -1792,7 +1792,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomRight" activeCell="E13" sqref="E13:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="12.75"/>
@@ -2045,13 +2045,13 @@
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="17" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17" t="s">
@@ -2063,13 +2063,11 @@
       <c r="I12" s="26"/>
       <c r="J12" s="39"/>
       <c r="K12" s="27"/>
-      <c r="L12" s="27" t="s">
-        <v>15</v>
-      </c>
+      <c r="L12" s="27"/>
     </row>
     <row r="13" ht="38.25" spans="1:12">
       <c r="A13" s="17" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>34</v>
@@ -2106,7 +2104,9 @@
         <v>41</v>
       </c>
       <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="E14" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
       <c r="H14" s="26"/>
@@ -2956,7 +2956,7 @@
   <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A59" sqref="A59:A61"/>
     </sheetView>

</xml_diff>

<commit_message>
sn: upate coverage form.
</commit_message>
<xml_diff>
--- a/Coverage Survey/Senegal/sn_sct_lf_2_couverture_202112.xlsx
+++ b/Coverage Survey/Senegal/sn_sct_lf_2_couverture_202112.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12345"/>
+    <workbookView windowWidth="28800" windowHeight="12345" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" iterate="1" iterateCount="1000" iterateDelta="0.001"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -543,7 +543,7 @@
     <t>3. Je ne suis pas malade</t>
   </si>
   <si>
-    <t>4.pas.recu.suffisamment.d’informations</t>
+    <t>4.pas.recu.suffisamment.d.informations</t>
   </si>
   <si>
     <t xml:space="preserve">4. Je n'ai pas eu suffisament d'informations sur le médicament </t>
@@ -674,12 +674,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -734,10 +734,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -748,10 +748,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -771,15 +772,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -793,16 +825,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -822,45 +853,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -869,20 +861,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="129"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -933,19 +926,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -957,31 +956,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -993,13 +968,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1011,7 +980,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1029,6 +1028,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1041,55 +1052,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1101,13 +1064,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1132,6 +1101,21 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1175,6 +1159,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1200,160 +1202,127 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1362,19 +1331,19 @@
     <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1387,7 +1356,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1425,9 +1394,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1787,7 +1753,7 @@
   </sheetPr>
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -1854,7 +1820,7 @@
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
       <c r="F2" s="14"/>
-      <c r="G2" s="24"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
@@ -1881,11 +1847,11 @@
       <c r="G3" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="15" t="s">
@@ -1903,11 +1869,11 @@
       </c>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="15" t="s">
@@ -1925,11 +1891,11 @@
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="15" t="s">
@@ -1947,11 +1913,11 @@
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="15"/>
@@ -1961,11 +1927,11 @@
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="16"/>
@@ -1989,11 +1955,11 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="26"/>
     </row>
     <row r="10" ht="38.25" spans="1:12">
       <c r="A10" s="17" t="s">
@@ -2013,11 +1979,11 @@
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="17" t="s">
@@ -2033,13 +1999,13 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="38" t="s">
+      <c r="H11" s="25"/>
+      <c r="I11" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="39"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27" t="s">
+      <c r="J11" s="38"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2059,11 +2025,11 @@
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
     </row>
     <row r="13" ht="38.25" spans="1:12">
       <c r="A13" s="17" t="s">
@@ -2087,11 +2053,11 @@
       <c r="G13" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="17" t="s">
@@ -2109,11 +2075,11 @@
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
     </row>
     <row r="15" s="9" customFormat="1" spans="1:12">
       <c r="A15" s="17"/>
@@ -2121,13 +2087,13 @@
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
     </row>
     <row r="16" s="10" customFormat="1" spans="1:12">
       <c r="A16" s="18" t="s">
@@ -2141,13 +2107,13 @@
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
     </row>
     <row r="17" s="10" customFormat="1" spans="1:12">
       <c r="A17" s="18"/>
@@ -2155,13 +2121,13 @@
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
     </row>
     <row r="18" s="10" customFormat="1" ht="25.5" spans="1:12">
       <c r="A18" s="18" t="s">
@@ -2177,13 +2143,13 @@
       <c r="E18" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
     </row>
     <row r="19" s="10" customFormat="1" ht="25.5" spans="1:12">
       <c r="A19" s="18" t="s">
@@ -2199,15 +2165,15 @@
       <c r="E19" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29" t="s">
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="I19" s="29"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
     </row>
     <row r="20" s="10" customFormat="1" ht="51" spans="1:12">
       <c r="A20" s="18" t="s">
@@ -2223,15 +2189,15 @@
       <c r="E20" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29" t="s">
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
     </row>
     <row r="21" s="10" customFormat="1" ht="25.5" spans="1:12">
       <c r="A21" s="18" t="s">
@@ -2247,15 +2213,15 @@
       <c r="E21" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="29" t="s">
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="I21" s="29"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
     </row>
     <row r="22" s="10" customFormat="1" ht="38.25" spans="1:12">
       <c r="A22" s="18" t="s">
@@ -2271,15 +2237,15 @@
       <c r="E22" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="29" t="s">
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="I22" s="29"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
     </row>
     <row r="23" s="10" customFormat="1" ht="51" spans="1:12">
       <c r="A23" s="18" t="s">
@@ -2295,15 +2261,15 @@
       <c r="E23" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="29" t="s">
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="I23" s="29"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
     </row>
     <row r="24" s="10" customFormat="1" ht="25.5" spans="1:12">
       <c r="A24" s="18" t="s">
@@ -2319,15 +2285,15 @@
       <c r="E24" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="29" t="s">
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="I24" s="29"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
     </row>
     <row r="25" s="10" customFormat="1" ht="38.25" spans="1:12">
       <c r="A25" s="18" t="s">
@@ -2343,15 +2309,15 @@
       <c r="E25" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="29" t="s">
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="I25" s="29"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
     </row>
     <row r="26" s="10" customFormat="1" spans="1:12">
       <c r="A26" s="18"/>
@@ -2359,13 +2325,13 @@
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
     </row>
     <row r="27" s="10" customFormat="1" spans="1:12">
       <c r="A27" s="18" t="s">
@@ -2375,13 +2341,13 @@
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="19"/>
@@ -2409,13 +2375,13 @@
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="30"/>
-      <c r="L29" s="30"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
     </row>
     <row r="30" s="11" customFormat="1" ht="25.5" spans="1:12">
       <c r="A30" s="20" t="s">
@@ -2431,13 +2397,13 @@
       <c r="E30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="30"/>
-      <c r="K30" s="30"/>
-      <c r="L30" s="30"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
     </row>
     <row r="31" s="11" customFormat="1" ht="25.5" spans="1:12">
       <c r="A31" s="20" t="s">
@@ -2453,15 +2419,15 @@
       <c r="E31" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="32" t="s">
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="I31" s="32"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="30"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
     </row>
     <row r="32" s="11" customFormat="1" ht="51" spans="1:12">
       <c r="A32" s="20" t="s">
@@ -2477,15 +2443,15 @@
       <c r="E32" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="32" t="s">
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="I32" s="32"/>
-      <c r="J32" s="30"/>
-      <c r="K32" s="30"/>
-      <c r="L32" s="30"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
     </row>
     <row r="33" s="11" customFormat="1" ht="25.5" spans="1:12">
       <c r="A33" s="20" t="s">
@@ -2501,15 +2467,15 @@
       <c r="E33" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="32" t="s">
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="I33" s="32"/>
-      <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
     </row>
     <row r="34" s="11" customFormat="1" ht="38.25" spans="1:12">
       <c r="A34" s="20" t="s">
@@ -2525,15 +2491,15 @@
       <c r="E34" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="32" t="s">
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="I34" s="32"/>
-      <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="30"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
     </row>
     <row r="35" s="11" customFormat="1" ht="51" spans="1:12">
       <c r="A35" s="20" t="s">
@@ -2549,15 +2515,15 @@
       <c r="E35" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="32" t="s">
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="I35" s="32"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
     </row>
     <row r="36" s="11" customFormat="1" ht="25.5" spans="1:12">
       <c r="A36" s="20" t="s">
@@ -2573,15 +2539,15 @@
       <c r="E36" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="32" t="s">
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="I36" s="32"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
     </row>
     <row r="37" s="11" customFormat="1" ht="38.25" spans="1:12">
       <c r="A37" s="20" t="s">
@@ -2597,15 +2563,15 @@
       <c r="E37" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="32" t="s">
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="I37" s="32"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
     </row>
     <row r="38" s="11" customFormat="1" spans="1:12">
       <c r="A38" s="20" t="s">
@@ -2615,13 +2581,13 @@
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="32"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="19"/>
@@ -2649,13 +2615,13 @@
       </c>
       <c r="D40" s="21"/>
       <c r="E40" s="21"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="33"/>
-      <c r="H40" s="34"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="33"/>
-      <c r="L40" s="33"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="32"/>
+      <c r="L40" s="32"/>
     </row>
     <row r="41" s="12" customFormat="1" ht="25.5" spans="1:12">
       <c r="A41" s="21" t="s">
@@ -2671,13 +2637,13 @@
       <c r="E41" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
-      <c r="H41" s="35"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="33"/>
-      <c r="K41" s="33"/>
-      <c r="L41" s="33"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="32"/>
     </row>
     <row r="42" s="12" customFormat="1" ht="25.5" spans="1:12">
       <c r="A42" s="21" t="s">
@@ -2693,15 +2659,15 @@
       <c r="E42" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F42" s="33"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="35" t="s">
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
+      <c r="H42" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="I42" s="35"/>
-      <c r="J42" s="33"/>
-      <c r="K42" s="33"/>
-      <c r="L42" s="33"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="32"/>
+      <c r="K42" s="32"/>
+      <c r="L42" s="32"/>
     </row>
     <row r="43" s="12" customFormat="1" ht="51" spans="1:12">
       <c r="A43" s="21" t="s">
@@ -2717,15 +2683,15 @@
       <c r="E43" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="35" t="s">
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="I43" s="35"/>
-      <c r="J43" s="33"/>
-      <c r="K43" s="33"/>
-      <c r="L43" s="33"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="32"/>
+      <c r="K43" s="32"/>
+      <c r="L43" s="32"/>
     </row>
     <row r="44" s="12" customFormat="1" ht="25.5" spans="1:12">
       <c r="A44" s="21" t="s">
@@ -2741,15 +2707,15 @@
       <c r="E44" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="35" t="s">
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="I44" s="35"/>
-      <c r="J44" s="33"/>
-      <c r="K44" s="33"/>
-      <c r="L44" s="33"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="32"/>
     </row>
     <row r="45" s="12" customFormat="1" ht="38.25" spans="1:12">
       <c r="A45" s="21" t="s">
@@ -2765,15 +2731,15 @@
       <c r="E45" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F45" s="33"/>
-      <c r="G45" s="33"/>
-      <c r="H45" s="35" t="s">
+      <c r="F45" s="32"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="I45" s="35"/>
-      <c r="J45" s="33"/>
-      <c r="K45" s="33"/>
-      <c r="L45" s="33"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
+      <c r="L45" s="32"/>
     </row>
     <row r="46" s="12" customFormat="1" ht="51" spans="1:12">
       <c r="A46" s="21" t="s">
@@ -2789,15 +2755,15 @@
       <c r="E46" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F46" s="33"/>
-      <c r="G46" s="33"/>
-      <c r="H46" s="35" t="s">
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="I46" s="35"/>
-      <c r="J46" s="33"/>
-      <c r="K46" s="33"/>
-      <c r="L46" s="33"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="32"/>
+      <c r="L46" s="32"/>
     </row>
     <row r="47" s="12" customFormat="1" ht="25.5" spans="1:12">
       <c r="A47" s="21" t="s">
@@ -2813,15 +2779,15 @@
       <c r="E47" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F47" s="33"/>
-      <c r="G47" s="33"/>
-      <c r="H47" s="35" t="s">
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="I47" s="35"/>
-      <c r="J47" s="33"/>
-      <c r="K47" s="33"/>
-      <c r="L47" s="33"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="32"/>
+      <c r="K47" s="32"/>
+      <c r="L47" s="32"/>
     </row>
     <row r="48" s="12" customFormat="1" ht="38.25" spans="1:12">
       <c r="A48" s="21" t="s">
@@ -2837,15 +2803,15 @@
       <c r="E48" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="35" t="s">
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
+      <c r="H48" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="I48" s="35"/>
-      <c r="J48" s="33"/>
-      <c r="K48" s="33"/>
-      <c r="L48" s="33"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="32"/>
+      <c r="K48" s="32"/>
+      <c r="L48" s="32"/>
     </row>
     <row r="49" s="12" customFormat="1" spans="1:12">
       <c r="A49" s="21" t="s">
@@ -2855,13 +2821,13 @@
       <c r="C49" s="21"/>
       <c r="D49" s="21"/>
       <c r="E49" s="21"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="35"/>
-      <c r="I49" s="35"/>
-      <c r="J49" s="33"/>
-      <c r="K49" s="33"/>
-      <c r="L49" s="33"/>
+      <c r="F49" s="32"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="34"/>
+      <c r="I49" s="34"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="32"/>
+      <c r="L49" s="32"/>
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="19"/>
@@ -2934,8 +2900,8 @@
       <c r="L53" s="16"/>
     </row>
     <row r="54" spans="2:3">
-      <c r="B54" s="23"/>
-      <c r="C54" s="23"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>
@@ -2955,10 +2921,10 @@
   </sheetPr>
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59:A61"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="12.75" outlineLevelCol="7"/>

</xml_diff>